<commit_message>
Update bulk upload template to use passport codes instead of player names
Refactors the bulk match upload process to utilize player passport codes for identification, updating both English and Chinese templates and the server-side route handler in `server/routes/admin-bulk-upload.ts` to reflect this change.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: afbfe8a0-c5d4-4dfd-9b58-5f6304cce5ca
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/7c53293f-df0f-44d1-aa13-74da41f82777/afbfe8a0-c5d4-4dfd-9b58-5f6304cce5ca/jvQz0dy
</commit_message>
<xml_diff>
--- a/bulk-match-template-bilingual-chinese.xlsx
+++ b/bulk-match-template-bilingual-chinese.xlsx
@@ -441,13 +441,13 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>张伟</v>
+        <v>HVGN0BW0</v>
       </c>
       <c r="B2" t="str">
         <v/>
       </c>
       <c r="C2" t="str">
-        <v>李娜</v>
+        <v>KGLE38K4</v>
       </c>
       <c r="D2" t="str">
         <v/>
@@ -467,16 +467,16 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>王强</v>
+        <v>MJST45X9</v>
       </c>
       <c r="B3" t="str">
-        <v>刘敏</v>
+        <v>SWQR78Z2</v>
       </c>
       <c r="C3" t="str">
-        <v>陈军</v>
+        <v>TBPL91M5</v>
       </c>
       <c r="D3" t="str">
-        <v>赵静</v>
+        <v>LCKM33Y8</v>
       </c>
       <c r="E3" t="str">
         <v>11</v>
@@ -493,13 +493,13 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>杨涛</v>
+        <v>DLVW67N4</v>
       </c>
       <c r="B4" t="str">
         <v/>
       </c>
       <c r="C4" t="str">
-        <v>孙丽</v>
+        <v>EDRX29H6</v>
       </c>
       <c r="D4" t="str">
         <v/>
@@ -514,21 +514,21 @@
         <v>2025-01-16</v>
       </c>
       <c r="H4" t="str">
-        <v>男</v>
+        <v>M</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>马飞</v>
+        <v>AWJF82P1</v>
       </c>
       <c r="B5" t="str">
-        <v>周芳</v>
+        <v>JLMN56Q3</v>
       </c>
       <c r="C5" t="str">
-        <v>吴斌</v>
+        <v>RZQW74T7</v>
       </c>
       <c r="D5" t="str">
-        <v>郑红</v>
+        <v>MKHY93V0</v>
       </c>
       <c r="E5" t="str">
         <v>11</v>
@@ -545,13 +545,13 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>林浩</v>
+        <v>CTBR48K5</v>
       </c>
       <c r="B6" t="str">
         <v/>
       </c>
       <c r="C6" t="str">
-        <v>黄艳</v>
+        <v>ARLZ61F9</v>
       </c>
       <c r="D6" t="str">
         <v/>
@@ -566,7 +566,7 @@
         <v>2025-01-17</v>
       </c>
       <c r="H6" t="str">
-        <v>女</v>
+        <v>F</v>
       </c>
     </row>
   </sheetData>
@@ -598,32 +598,32 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>1. 使用已注册的用户名或护照码填写球员姓名</v>
+        <v>格式指南：</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>2. 单打比赛时，第二个球员栏位留空</v>
+        <v>• 使用选手护照代码（例如：HVGN0BW0, KGLE38K4）</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>3. 比分格式：11、9、13等</v>
+        <v>• 单打比赛请将第一队选手二和第二队选手二留空</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>4. 日期格式：YYYY-MM-DD（例：2025-01-15）</v>
+        <v>• 使用如下分数格式：11, 7, 15, 13（游戏比分）</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>5. 性别覆盖：留空自动检测，使用 男/女 进行覆盖</v>
+        <v>• 日期格式：YYYY-MM-DD（例如：2025-01-15）</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>6. 上传时保存为 .xlsx 文件</v>
+        <v>• 性别覆盖：男或女（可选，用于跨性别比赛）</v>
       </c>
     </row>
     <row r="9">
@@ -633,47 +633,47 @@
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>列详情：</v>
+        <v>示例：</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>- 第一队选手一：必填 - 第一队的第一位球员</v>
+        <v>单打：HVGN0BW0 对 KGLE38K4，比分 11-7</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>- 第一队选手二：选填 - 双打的第二位球员（单打留空）</v>
+        <v>双打：MJST45X9/SWQR78Z2 对 TBPL91M5/LCKM33Y8，比分 11-9</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>- 第二队选手一：必填 - 第二队的第一位球员</v>
+        <v/>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>- 第二队选手二：选填 - 双打的第二位球员（单打留空）</v>
+        <v>验证将检查：</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>- 第一队得分：必填 - 第一队的最终得分</v>
+        <v>• 所有护照代码在系统中存在</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>- 第二队得分：必填 - 第二队的最终得分</v>
+        <v>• 有效的分数格式</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>- 比赛日期：必填 - YYYY-MM-DD 格式的比赛日期</v>
+        <v>• 无重复比赛</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>- 性别覆盖：选填 - 男代表全男性比赛，女代表全女性比赛</v>
+        <v>• 正确的日期格式</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update bulk upload template to use passport codes for player identification
Modify the admin bulk upload template and headers to require passport codes instead of player names for enhanced data accuracy and clarity. Adjust column widths for new headers.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: afbfe8a0-c5d4-4dfd-9b58-5f6304cce5ca
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/7c53293f-df0f-44d1-aa13-74da41f82777/afbfe8a0-c5d4-4dfd-9b58-5f6304cce5ca/jvQz0dy
</commit_message>
<xml_diff>
--- a/bulk-match-template-bilingual-chinese.xlsx
+++ b/bulk-match-template-bilingual-chinese.xlsx
@@ -403,10 +403,10 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="32.83203125" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" customWidth="1"/>
-    <col min="3" max="3" width="32.83203125" customWidth="1"/>
-    <col min="4" max="4" width="32.83203125" customWidth="1"/>
+    <col min="1" max="1" width="40.83203125" customWidth="1"/>
+    <col min="2" max="2" width="40.83203125" customWidth="1"/>
+    <col min="3" max="3" width="40.83203125" customWidth="1"/>
+    <col min="4" max="4" width="40.83203125" customWidth="1"/>
     <col min="5" max="5" width="20.83203125" customWidth="1"/>
     <col min="6" max="6" width="20.83203125" customWidth="1"/>
     <col min="7" max="7" width="18.83203125" customWidth="1"/>
@@ -415,16 +415,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Team_1_Player_1 / 第一队选手一</v>
+        <v>Team_1_Player_1_Passport / 第一队选手一护照码</v>
       </c>
       <c r="B1" t="str">
-        <v>Team_1_Player_2 / 第一队选手二</v>
+        <v>Team_1_Player_2_Passport / 第一队选手二护照码</v>
       </c>
       <c r="C1" t="str">
-        <v>Team_2_Player_1 / 第二队选手一</v>
+        <v>Team_2_Player_1_Passport / 第二队选手一护照码</v>
       </c>
       <c r="D1" t="str">
-        <v>Team_2_Player_2 / 第二队选手二</v>
+        <v>Team_2_Player_2_Passport / 第二队选手二护照码</v>
       </c>
       <c r="E1" t="str">
         <v>Team_1_Score / 第一队得分</v>
@@ -578,7 +578,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A18"/>
+  <dimension ref="A1:A23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -603,12 +603,12 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>• 使用选手护照代码（例如：HVGN0BW0, KGLE38K4）</v>
+        <v>• 使用选手护照代码（例如：HVGN0BW0, KGLE38K4）- 不是姓名</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>• 单打比赛请将第一队选手二和第二队选手二留空</v>
+        <v>• 单打比赛请将第一队选手二护照码和第二队选手二护照码留空</v>
       </c>
     </row>
     <row r="6">
@@ -653,32 +653,57 @@
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>验证将检查：</v>
+        <v>重要提示 - 仅使用护照代码：</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>• 所有护照代码在系统中存在</v>
+        <v>• 系统要求护照代码，不是选手姓名</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>• 有效的分数格式</v>
+        <v>• 每个护照代码为8个字符（字母和数字）</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>• 无重复比赛</v>
+        <v>• 从选手档案或管理面板查找护照代码</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>验证将检查：</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>• 所有护照代码在系统中存在</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>• 有效的分数格式</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>• 无重复比赛</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
         <v>• 正确的日期格式</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:A18"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:A23"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>